<commit_message>
add 1.1 version of vocabularies to imports
</commit_message>
<xml_diff>
--- a/storage/app/keywords/1-1/230323 MSL vocabulary Geochemistry.xlsx
+++ b/storage/app/keywords/1-1/230323 MSL vocabulary Geochemistry.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/r_p_j_pijnenburg_uu_nl/Documents/EPOS-NL/07 Data/Metadata/230323 update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\epos\storage\app\keywords\1-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{FA7D9FDB-6B06-42E3-865F-9A1FB45F6CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D78893C-01AC-4837-94EC-0C8EBECC6311}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE314C-0F6E-444A-AE60-7F744B7BB6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="2" xr2:uid="{F3BCA07C-F085-4C2E-91D1-BE33B4A72469}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="1" activeTab="2" xr2:uid="{F3BCA07C-F085-4C2E-91D1-BE33B4A72469}"/>
   </bookViews>
   <sheets>
     <sheet name="NB" sheetId="4" r:id="rId1"/>
-    <sheet name="Measurement technique" sheetId="3" r:id="rId2"/>
-    <sheet name="Measured property" sheetId="1" r:id="rId3"/>
+    <sheet name="Technique" sheetId="3" r:id="rId2"/>
+    <sheet name="Measured property #parameter" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2406,7 +2406,7 @@
       <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -2455,15 +2455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC320CFB-F604-4B25-9FB7-E194056F8F60}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="71.44140625" customWidth="1"/>
+    <col min="3" max="3" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2510,7 +2510,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3">
       <c r="A7" s="10"/>
       <c r="B7" s="8" t="s">
         <v>581</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" ht="15">
+    <row r="9" spans="1:3">
       <c r="A9" s="10"/>
       <c r="B9" s="8" t="s">
         <v>543</v>
@@ -2536,7 +2536,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>8</v>
@@ -2760,43 +2760,43 @@
         <v>558</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15">
+    <row r="55" spans="1:3">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15">
+    <row r="56" spans="1:3">
       <c r="A56" s="1"/>
       <c r="C56" s="8" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15">
+    <row r="57" spans="1:3">
       <c r="A57" s="1"/>
       <c r="C57" s="8" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15">
+    <row r="58" spans="1:3">
       <c r="A58" s="1"/>
       <c r="C58" s="8" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15">
+    <row r="59" spans="1:3">
       <c r="A59" s="1"/>
       <c r="C59" s="8" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15">
+    <row r="60" spans="1:3">
       <c r="A60" s="1"/>
       <c r="C60" s="8" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15">
+    <row r="61" spans="1:3">
       <c r="A61" s="1"/>
       <c r="C61" s="8" t="s">
         <v>564</v>
@@ -2984,19 +2984,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5493FE-C873-4AB4-80C7-643EAFBCE7F0}">
   <dimension ref="A1:D566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="62.6640625" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" customHeight="1">
+    <row r="1" spans="1:4" ht="14.45" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
         <v>622</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="13.95" customHeight="1">
+    <row r="128" spans="1:2" ht="13.9" customHeight="1">
       <c r="A128" t="s">
         <v>111</v>
       </c>
@@ -5787,10 +5787,10 @@
     <row r="564" spans="2:4" ht="18" customHeight="1">
       <c r="D564" s="6"/>
     </row>
-    <row r="565" spans="2:4" ht="16.95" customHeight="1">
+    <row r="565" spans="2:4" ht="16.899999999999999" customHeight="1">
       <c r="D565" s="6"/>
     </row>
-    <row r="566" spans="2:4" ht="16.2" customHeight="1">
+    <row r="566" spans="2:4" ht="16.149999999999999" customHeight="1">
       <c r="D566" s="6"/>
     </row>
   </sheetData>
@@ -6045,5 +6045,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E02C56-12D8-4A0F-900C-B240A6919123}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E02C56-12D8-4A0F-900C-B240A6919123}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
+    <ds:schemaRef ds:uri="53df6a5f-9334-4503-a845-5e05459a4c71"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>